<commit_message>
Actualizacion herramientas de exploracion
</commit_message>
<xml_diff>
--- a/resources/import_templates/f02_estudiantes.xlsx
+++ b/resources/import_templates/f02_estudiantes.xlsx
@@ -8,13 +8,95 @@
   </bookViews>
   <sheets>
     <sheet name="estudiantes" sheetId="1" r:id="rId1"/>
+    <sheet name="referencia" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DeKinder:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Utilice el código que puede ver en la hoja "referencia".
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">DeKinder: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Utilice el código que puede ver en la hoja "referencia".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DeKinder:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Busca el ID del grupo en el listado de exploración de grupos.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Nombres</t>
   </si>
@@ -22,18 +104,6 @@
     <t>Apellidos</t>
   </si>
   <si>
-    <t>Jaramillo</t>
-  </si>
-  <si>
-    <t>Correa</t>
-  </si>
-  <si>
-    <t>Jimena</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
     <t>Sexo</t>
   </si>
   <si>
@@ -52,20 +122,56 @@
     <t>Fecha nacimiento</t>
   </si>
   <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Javier</t>
-  </si>
-  <si>
-    <t>Ojeda</t>
+    <t>Salomé</t>
+  </si>
+  <si>
+    <t>López Jurado</t>
+  </si>
+  <si>
+    <t>Lorenzo</t>
+  </si>
+  <si>
+    <t>Correa Marín</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Díaz Niño</t>
+  </si>
+  <si>
+    <t>Cod Tipo Documento</t>
+  </si>
+  <si>
+    <t>Cod Sexo</t>
+  </si>
+  <si>
+    <t>Cédula de ciudadanía</t>
+  </si>
+  <si>
+    <t>Cédula de extranjería</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>Tarjeta de Identidad</t>
+  </si>
+  <si>
+    <t>Registro Civil</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Hombre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +187,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +232,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -126,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,11 +575,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +587,10 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -476,33 +602,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>748596</v>
+        <v>1014789456</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -514,21 +640,21 @@
         <v>42005</v>
       </c>
       <c r="G2">
-        <v>123456987</v>
+        <v>102030</v>
       </c>
       <c r="H2">
-        <v>10035</v>
+        <v>10048</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>123456798</v>
+        <v>1014987412</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -540,18 +666,21 @@
         <v>42098</v>
       </c>
       <c r="G3">
-        <v>987654321</v>
+        <v>102031</v>
       </c>
       <c r="H3">
-        <v>10035</v>
+        <v>10048</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="C4">
-        <v>987987654</v>
+        <v>1014456963</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -563,36 +692,97 @@
         <v>42099</v>
       </c>
       <c r="G4">
-        <v>987654654</v>
+        <v>102032</v>
       </c>
       <c r="H4">
-        <v>10035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10048</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>16073346</v>
-      </c>
-      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6">
         <v>6</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5">
-        <v>30115</v>
-      </c>
-      <c r="G5">
-        <v>82061303606</v>
-      </c>
-      <c r="H5">
-        <v>10035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>